<commit_message>
added map ccords for each kill
</commit_message>
<xml_diff>
--- a/app/data_final0.xlsx
+++ b/app/data_final0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Joueur</t>
   </si>
@@ -46,55 +46,58 @@
     <t>KD</t>
   </si>
   <si>
-    <t>Saysum</t>
-  </si>
-  <si>
-    <t>YelazZ</t>
+    <t>Hîstorîa</t>
+  </si>
+  <si>
+    <t>mommy cat</t>
   </si>
   <si>
     <t>Zeddxx</t>
   </si>
   <si>
-    <t>Anevrysme</t>
-  </si>
-  <si>
-    <t>FRÊÊ</t>
-  </si>
-  <si>
-    <t>Simoflipe</t>
-  </si>
-  <si>
-    <t>keshilolz</t>
-  </si>
-  <si>
-    <t>Oréwa</t>
-  </si>
-  <si>
-    <t>Sphenks</t>
-  </si>
-  <si>
-    <t>i  Z  k  i</t>
+    <t>xiiixo</t>
+  </si>
+  <si>
+    <t>XENOX</t>
+  </si>
+  <si>
+    <t>Faizenissobad</t>
+  </si>
+  <si>
+    <t>DrLimits</t>
+  </si>
+  <si>
+    <t>Lazar</t>
+  </si>
+  <si>
+    <t>Bones Slayer Zed</t>
+  </si>
+  <si>
+    <t>fenix3006</t>
+  </si>
+  <si>
+    <t>Raze</t>
+  </si>
+  <si>
+    <t>Sage</t>
   </si>
   <si>
     <t>Reyna</t>
   </si>
   <si>
-    <t>Killjoy</t>
-  </si>
-  <si>
-    <t>Cypher</t>
+    <t>Sova</t>
   </si>
   <si>
     <t>Chamber</t>
   </si>
   <si>
-    <t>Yoru</t>
+    <t>Neon</t>
+  </si>
+  <si>
+    <t>Brimstone</t>
   </si>
   <si>
     <t>Jett</t>
-  </si>
-  <si>
-    <t>Sova</t>
   </si>
 </sst>
 </file>
@@ -501,28 +504,28 @@
         <v>20</v>
       </c>
       <c r="D2">
-        <v>6204</v>
+        <v>2336</v>
       </c>
       <c r="E2">
-        <v>3882</v>
+        <v>1739</v>
       </c>
       <c r="F2">
-        <v>3905</v>
+        <v>2847</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="I2">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2">
-        <v>1.157894736842105</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -536,28 +539,28 @@
         <v>21</v>
       </c>
       <c r="D3">
-        <v>2506</v>
+        <v>4716</v>
       </c>
       <c r="E3">
-        <v>1672</v>
+        <v>2836</v>
       </c>
       <c r="F3">
-        <v>3842</v>
+        <v>3269</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H3">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I3">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0.2916666666666667</v>
+        <v>0.9411764705882353</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -571,28 +574,28 @@
         <v>22</v>
       </c>
       <c r="D4">
-        <v>6776</v>
+        <v>6634</v>
       </c>
       <c r="E4">
-        <v>4736</v>
+        <v>3749</v>
       </c>
       <c r="F4">
-        <v>4083</v>
+        <v>2258</v>
       </c>
       <c r="G4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H4">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I4">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>1.375</v>
+        <v>2.083333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -603,31 +606,31 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>7914</v>
+        <v>4085</v>
       </c>
       <c r="E5">
-        <v>5152</v>
+        <v>2406</v>
       </c>
       <c r="F5">
-        <v>3459</v>
+        <v>2645</v>
       </c>
       <c r="G5">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="I5">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>1.333333333333333</v>
+        <v>0.9333333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -638,31 +641,31 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6">
-        <v>4922</v>
+        <v>4540</v>
       </c>
       <c r="E6">
-        <v>3198</v>
+        <v>2820</v>
       </c>
       <c r="F6">
-        <v>3091</v>
+        <v>2768</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H6">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K6">
-        <v>1.266666666666667</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -673,31 +676,31 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>2256</v>
+        <v>5140</v>
       </c>
       <c r="E7">
-        <v>1593</v>
+        <v>3465</v>
       </c>
       <c r="F7">
-        <v>3395</v>
+        <v>2989</v>
       </c>
       <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>19</v>
+      </c>
+      <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
         <v>4</v>
       </c>
-      <c r="H7">
-        <v>7</v>
-      </c>
-      <c r="I7">
-        <v>20</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
       <c r="K7">
-        <v>0.35</v>
+        <v>1.266666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -711,28 +714,28 @@
         <v>25</v>
       </c>
       <c r="D8">
-        <v>6031</v>
+        <v>2243</v>
       </c>
       <c r="E8">
-        <v>5049</v>
+        <v>1660</v>
       </c>
       <c r="F8">
-        <v>4119</v>
+        <v>2780</v>
       </c>
       <c r="G8">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I8">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>1.052631578947368</v>
+        <v>0.3529411764705883</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -743,31 +746,31 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D9">
-        <v>9419</v>
+        <v>3933</v>
       </c>
       <c r="E9">
-        <v>5640</v>
+        <v>2743</v>
       </c>
       <c r="F9">
-        <v>3499</v>
+        <v>2694</v>
       </c>
       <c r="G9">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H9">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="I9">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K9">
-        <v>1.882352941176471</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -778,31 +781,31 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>3217</v>
+        <v>4038</v>
       </c>
       <c r="E10">
-        <v>2077</v>
+        <v>2444</v>
       </c>
       <c r="F10">
-        <v>3328</v>
+        <v>2397</v>
       </c>
       <c r="G10">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10">
         <v>12</v>
-      </c>
-      <c r="I10">
-        <v>17</v>
       </c>
       <c r="J10">
         <v>2</v>
       </c>
       <c r="K10">
-        <v>0.7058823529411765</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -813,31 +816,31 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D11">
-        <v>5094</v>
+        <v>4969</v>
       </c>
       <c r="E11">
-        <v>2890</v>
+        <v>3010</v>
       </c>
       <c r="F11">
-        <v>3434</v>
+        <v>3067</v>
       </c>
       <c r="G11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H11">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I11">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J11">
         <v>3</v>
       </c>
       <c r="K11">
-        <v>0.9473684210526315</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>